<commit_message>
Updated gold map docs.
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7FA646-61E9-4AA9-AAF6-0CE46315D373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBECAEB-B070-4E55-8EAE-54E5AAC7C9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14710" yWindow="8530" windowWidth="23580" windowHeight="11980" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" firstSheet="1" activeTab="4" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
-    <sheet name="Herd" sheetId="7" r:id="rId2"/>
-    <sheet name="Party" sheetId="8" r:id="rId3"/>
-    <sheet name="Site Party" sheetId="9" r:id="rId4"/>
+    <sheet name="Party" sheetId="8" r:id="rId2"/>
+    <sheet name="Site Party Role Relations" sheetId="9" r:id="rId3"/>
+    <sheet name="Site Group Mark Relations" sheetId="7" r:id="rId4"/>
     <sheet name="LOVs Required" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
     <author>MarkGent1</author>
   </authors>
   <commentList>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{45241C45-117A-4C12-8C72-DF3C6608B198}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{7BC1F4FC-3C9E-40F9-8D60-11A815EAD5A4}">
       <text>
         <r>
           <rPr>
@@ -42,7 +42,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>MarkGent1:</t>
         </r>
@@ -51,14 +51,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-HoldingNumber</t>
+Person
+Company</t>
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{3C19AE7A-114A-47EF-8496-C93E5FD3692C}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{07698770-79F3-497B-9C9E-FA04CE333F61}">
       <text>
         <r>
           <rPr>
@@ -66,7 +67,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>MarkGent1:</t>
         </r>
@@ -75,11 +76,11 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Person
-Company</t>
+SAM
+CTS</t>
         </r>
       </text>
     </comment>
@@ -113,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="230">
   <si>
     <t>Source</t>
   </si>
@@ -124,9 +125,6 @@
     <t>LastUpdatedBatchId</t>
   </si>
   <si>
-    <t>CountyParishHoldingNumber</t>
-  </si>
-  <si>
     <t>CphTypeIdentifier</t>
   </si>
   <si>
@@ -142,9 +140,6 @@
     <t>Location.Address.AddressLine</t>
   </si>
   <si>
-    <t>LocationName</t>
-  </si>
-  <si>
     <t>Location.Address.AddressLocality</t>
   </si>
   <si>
@@ -247,9 +242,6 @@
     <t>H1000001</t>
   </si>
   <si>
-    <t>GroupMark.GroupMark</t>
-  </si>
-  <si>
     <t>ProductionUsageId</t>
   </si>
   <si>
@@ -277,9 +269,6 @@
     <t>ProductionUsageCode</t>
   </si>
   <si>
-    <t>TbTestingIntervalId</t>
-  </si>
-  <si>
     <t>GroupMarkStartDate</t>
   </si>
   <si>
@@ -292,12 +281,6 @@
     <t>1-3, 10-12</t>
   </si>
   <si>
-    <t>GroupMarkDocument</t>
-  </si>
-  <si>
-    <t>6 Months</t>
-  </si>
-  <si>
     <t>SamPartyDocument</t>
   </si>
   <si>
@@ -430,9 +413,6 @@
     <t>20000000-0000-0000-0000-000000000002</t>
   </si>
   <si>
-    <t>IdentifierType</t>
-  </si>
-  <si>
     <t>Enum or string value</t>
   </si>
   <si>
@@ -529,33 +509,12 @@
     <t>true</t>
   </si>
   <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <t>Species[].Id</t>
-  </si>
-  <si>
-    <t>Species[].Code</t>
-  </si>
-  <si>
-    <t>Species[].Name</t>
-  </si>
-  <si>
     <t>BV</t>
   </si>
   <si>
     <t>Bovine (Cattle)</t>
   </si>
   <si>
-    <t>Marks[].Mark</t>
-  </si>
-  <si>
-    <t>Marks[].StartDate</t>
-  </si>
-  <si>
-    <t>Marks[].EndDate</t>
-  </si>
-  <si>
     <t>PartyTypeId</t>
   </si>
   <si>
@@ -682,12 +641,6 @@
     <t>PartyRoles[].SpeciesManagedByRole[].EndDate</t>
   </si>
   <si>
-    <t>SitePartyDocument</t>
-  </si>
-  <si>
-    <t>SamPartyDocument &amp; PartyRoleRelationshipDocument</t>
-  </si>
-  <si>
     <t>RoleTypeId</t>
   </si>
   <si>
@@ -695,13 +648,169 @@
   </si>
   <si>
     <t>EffectiveToData</t>
+  </si>
+  <si>
+    <t>Location.Address.CountrySubDivision</t>
+  </si>
+  <si>
+    <t>DiseaseType</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>IntervalUnitOfTime</t>
+  </si>
+  <si>
+    <t>CphRelationshipType</t>
+  </si>
+  <si>
+    <t>PremiseSubActivityTypeCode</t>
+  </si>
+  <si>
+    <t>MovementRestrictionReasonCode</t>
+  </si>
+  <si>
+    <t>ProductionUsageCodeList</t>
+  </si>
+  <si>
+    <t>SpeciesTypeCode *</t>
+  </si>
+  <si>
+    <t>SecondaryCph *</t>
+  </si>
+  <si>
+    <t>LocationName *</t>
+  </si>
+  <si>
+    <t>CountyParishHoldingNumber *</t>
+  </si>
+  <si>
+    <t>SiteIdentifierType</t>
+  </si>
+  <si>
+    <t>PartyInitials</t>
+  </si>
+  <si>
+    <t>Address.CountrySubDivision</t>
+  </si>
+  <si>
+    <t>IsHolder</t>
+  </si>
+  <si>
+    <t>HoldingIdentifier</t>
+  </si>
+  <si>
+    <t>HoldingIdentifierType</t>
+  </si>
+  <si>
+    <t>RoleTypeName</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole</t>
+  </si>
+  <si>
+    <t>SitePartyRoleRelationshipDocument</t>
+  </si>
+  <si>
+    <t>SourceRoleName</t>
+  </si>
+  <si>
+    <t>CphNumber</t>
+  </si>
+  <si>
+    <t>LivestockKeeper</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].Id</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].Code</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].Name</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].StartDate</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].EndDate</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].SpeciesTypeCode</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].SpeciesTypeName</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].SpeciesTypeId</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].SpeciesTypeId</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].GroupMarkStartDate</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].GroupMarkEndDate</t>
+  </si>
+  <si>
+    <t>DERIVED DATA</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Herdmark</t>
+  </si>
+  <si>
+    <t>CountyParishHoldingHerd</t>
+  </si>
+  <si>
+    <t>PartyId *</t>
+  </si>
+  <si>
+    <t>HoldingIdentifier *</t>
+  </si>
+  <si>
+    <t>RoleTypeId *</t>
+  </si>
+  <si>
+    <t>IsHolder *</t>
+  </si>
+  <si>
+    <t>Herdmark *</t>
+  </si>
+  <si>
+    <t>CountyParishHoldingHerd *</t>
+  </si>
+  <si>
+    <t>12/345/6789/01</t>
+  </si>
+  <si>
+    <t>SiteGroupMarkRelationshipDocument</t>
+  </si>
+  <si>
+    <t>SamHerdDocument</t>
+  </si>
+  <si>
+    <t>ProductionUsageId *</t>
+  </si>
+  <si>
+    <t>Derived by Party Roles from matching Herds</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Months</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -758,17 +867,27 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -818,7 +937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -871,6 +990,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1187,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1212,19 +1346,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -1236,33 +1370,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1280,431 +1414,531 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
+      <c r="A8" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
+      <c r="A10" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>37</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E17" s="18"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>32</v>
-      </c>
+    <row r="18" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="B19" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="6"/>
+        <v>121</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F19" s="7" t="s">
-        <v>134</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="4">
-        <v>25962203</v>
-      </c>
-      <c r="F24" s="4">
-        <v>25962203</v>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="E25" s="4">
-        <v>399568</v>
+        <v>25962203</v>
       </c>
       <c r="F25" s="4">
-        <v>399568</v>
+        <v>25962203</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E26" s="4">
-        <v>579087</v>
+        <v>399568</v>
       </c>
       <c r="F26" s="4">
-        <v>579087</v>
+        <v>399568</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="E27" s="4">
+        <v>579087</v>
+      </c>
+      <c r="F27" s="4">
+        <v>579087</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>20</v>
+        <v>180</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>39</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E30" s="18"/>
       <c r="F30" s="18"/>
     </row>
-    <row r="31" spans="1:6" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="E31" s="7" t="s">
+    <row r="31" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="F32" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:6" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="B41" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="3" t="s">
+    </row>
+    <row r="44" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="F47" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B37" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
-      <c r="B38" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="42" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="7"/>
-    </row>
-    <row r="44" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F44" s="7"/>
-    </row>
-    <row r="47" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="6"/>
+      <c r="B48" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+    </row>
+    <row r="52" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F52" s="7"/>
+    </row>
+    <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F54" s="7"/>
+    </row>
+    <row r="57" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F57" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1712,400 +1946,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF6CC05-8C87-45EE-8114-6B59C4D3ABC0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C839C088-4F6A-415F-B277-CCE418652376}">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="36.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="39.26953125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="38.81640625" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="37.54296875" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="E2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="11"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="11"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="9"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="E6" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C839C088-4F6A-415F-B277-CCE418652376}">
-  <dimension ref="A1:F40"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33:F34"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2127,19 +1972,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -2151,33 +1996,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2190,7 +2035,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -2203,471 +2048,491 @@
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>76</v>
-      </c>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>78</v>
+      <c r="E16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>167</v>
+      <c r="A17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>58</v>
+      <c r="E17" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>168</v>
+      <c r="A18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>90</v>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7" t="s">
-        <v>134</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="B25" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25" s="7"/>
+        <v>158</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F25" s="7" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="4">
+        <v>25962203</v>
+      </c>
+      <c r="F31" s="4">
+        <v>25962203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="4">
-        <v>25962203</v>
-      </c>
-      <c r="F29" s="4">
-        <v>25962203</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="E31" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
+      <c r="B32" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="E33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="E34" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="B35" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="6" t="s">
-        <v>142</v>
+        <v>167</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="E36" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B37" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B39" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B40" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>35</v>
+        <v>170</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B41" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E6 E15:F15" numberStoredAsText="1"/>
+    <ignoredError sqref="E6 E16:F16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA66AAD5-BDC2-41E6-A820-5F761A54ABFC}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A14" sqref="A14:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.6328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="58.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.08984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="36.36328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.08984375" style="3" customWidth="1"/>
     <col min="4" max="4" width="3.1796875" style="3" customWidth="1"/>
     <col min="5" max="5" width="36.6328125" style="4" customWidth="1"/>
     <col min="6" max="6" width="36.26953125" style="3" customWidth="1"/>
@@ -2682,19 +2547,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -2706,33 +2571,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2745,7 +2610,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -2757,59 +2622,233 @@
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>64</v>
+      <c r="A8" s="11" t="s">
+        <v>217</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="E9" s="7" t="s">
+    <row r="11" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F17" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>35</v>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2820,12 +2859,442 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF6CC05-8C87-45EE-8114-6B59C4D3ABC0}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.6328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="2.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="38.81640625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="37.54296875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="E2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E6 E24:F24" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454A6389-3CAC-4BFC-B100-395F08EF1093}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2836,94 +3305,102 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -2931,10 +3408,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validate extended data attribute maps for gold data maps (#44)
* Updated gold map docs.

* Minor to trigger pipeline.

* Fixed renaming issue with holding identifier

---------

Co-authored-by: Mark Gent <Mark.Gent@homesengland.gov.uk>
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7FA646-61E9-4AA9-AAF6-0CE46315D373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBECAEB-B070-4E55-8EAE-54E5AAC7C9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14710" yWindow="8530" windowWidth="23580" windowHeight="11980" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" firstSheet="1" activeTab="4" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
-    <sheet name="Herd" sheetId="7" r:id="rId2"/>
-    <sheet name="Party" sheetId="8" r:id="rId3"/>
-    <sheet name="Site Party" sheetId="9" r:id="rId4"/>
+    <sheet name="Party" sheetId="8" r:id="rId2"/>
+    <sheet name="Site Party Role Relations" sheetId="9" r:id="rId3"/>
+    <sheet name="Site Group Mark Relations" sheetId="7" r:id="rId4"/>
     <sheet name="LOVs Required" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
     <author>MarkGent1</author>
   </authors>
   <commentList>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{45241C45-117A-4C12-8C72-DF3C6608B198}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{7BC1F4FC-3C9E-40F9-8D60-11A815EAD5A4}">
       <text>
         <r>
           <rPr>
@@ -42,7 +42,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>MarkGent1:</t>
         </r>
@@ -51,14 +51,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-HoldingNumber</t>
+Person
+Company</t>
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{3C19AE7A-114A-47EF-8496-C93E5FD3692C}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{07698770-79F3-497B-9C9E-FA04CE333F61}">
       <text>
         <r>
           <rPr>
@@ -66,7 +67,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>MarkGent1:</t>
         </r>
@@ -75,11 +76,11 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Person
-Company</t>
+SAM
+CTS</t>
         </r>
       </text>
     </comment>
@@ -113,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="230">
   <si>
     <t>Source</t>
   </si>
@@ -124,9 +125,6 @@
     <t>LastUpdatedBatchId</t>
   </si>
   <si>
-    <t>CountyParishHoldingNumber</t>
-  </si>
-  <si>
     <t>CphTypeIdentifier</t>
   </si>
   <si>
@@ -142,9 +140,6 @@
     <t>Location.Address.AddressLine</t>
   </si>
   <si>
-    <t>LocationName</t>
-  </si>
-  <si>
     <t>Location.Address.AddressLocality</t>
   </si>
   <si>
@@ -247,9 +242,6 @@
     <t>H1000001</t>
   </si>
   <si>
-    <t>GroupMark.GroupMark</t>
-  </si>
-  <si>
     <t>ProductionUsageId</t>
   </si>
   <si>
@@ -277,9 +269,6 @@
     <t>ProductionUsageCode</t>
   </si>
   <si>
-    <t>TbTestingIntervalId</t>
-  </si>
-  <si>
     <t>GroupMarkStartDate</t>
   </si>
   <si>
@@ -292,12 +281,6 @@
     <t>1-3, 10-12</t>
   </si>
   <si>
-    <t>GroupMarkDocument</t>
-  </si>
-  <si>
-    <t>6 Months</t>
-  </si>
-  <si>
     <t>SamPartyDocument</t>
   </si>
   <si>
@@ -430,9 +413,6 @@
     <t>20000000-0000-0000-0000-000000000002</t>
   </si>
   <si>
-    <t>IdentifierType</t>
-  </si>
-  <si>
     <t>Enum or string value</t>
   </si>
   <si>
@@ -529,33 +509,12 @@
     <t>true</t>
   </si>
   <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <t>Species[].Id</t>
-  </si>
-  <si>
-    <t>Species[].Code</t>
-  </si>
-  <si>
-    <t>Species[].Name</t>
-  </si>
-  <si>
     <t>BV</t>
   </si>
   <si>
     <t>Bovine (Cattle)</t>
   </si>
   <si>
-    <t>Marks[].Mark</t>
-  </si>
-  <si>
-    <t>Marks[].StartDate</t>
-  </si>
-  <si>
-    <t>Marks[].EndDate</t>
-  </si>
-  <si>
     <t>PartyTypeId</t>
   </si>
   <si>
@@ -682,12 +641,6 @@
     <t>PartyRoles[].SpeciesManagedByRole[].EndDate</t>
   </si>
   <si>
-    <t>SitePartyDocument</t>
-  </si>
-  <si>
-    <t>SamPartyDocument &amp; PartyRoleRelationshipDocument</t>
-  </si>
-  <si>
     <t>RoleTypeId</t>
   </si>
   <si>
@@ -695,13 +648,169 @@
   </si>
   <si>
     <t>EffectiveToData</t>
+  </si>
+  <si>
+    <t>Location.Address.CountrySubDivision</t>
+  </si>
+  <si>
+    <t>DiseaseType</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>IntervalUnitOfTime</t>
+  </si>
+  <si>
+    <t>CphRelationshipType</t>
+  </si>
+  <si>
+    <t>PremiseSubActivityTypeCode</t>
+  </si>
+  <si>
+    <t>MovementRestrictionReasonCode</t>
+  </si>
+  <si>
+    <t>ProductionUsageCodeList</t>
+  </si>
+  <si>
+    <t>SpeciesTypeCode *</t>
+  </si>
+  <si>
+    <t>SecondaryCph *</t>
+  </si>
+  <si>
+    <t>LocationName *</t>
+  </si>
+  <si>
+    <t>CountyParishHoldingNumber *</t>
+  </si>
+  <si>
+    <t>SiteIdentifierType</t>
+  </si>
+  <si>
+    <t>PartyInitials</t>
+  </si>
+  <si>
+    <t>Address.CountrySubDivision</t>
+  </si>
+  <si>
+    <t>IsHolder</t>
+  </si>
+  <si>
+    <t>HoldingIdentifier</t>
+  </si>
+  <si>
+    <t>HoldingIdentifierType</t>
+  </si>
+  <si>
+    <t>RoleTypeName</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole</t>
+  </si>
+  <si>
+    <t>SitePartyRoleRelationshipDocument</t>
+  </si>
+  <si>
+    <t>SourceRoleName</t>
+  </si>
+  <si>
+    <t>CphNumber</t>
+  </si>
+  <si>
+    <t>LivestockKeeper</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].Id</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].Code</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].Name</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].StartDate</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].EndDate</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].SpeciesTypeCode</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].SpeciesTypeName</t>
+  </si>
+  <si>
+    <t>SpeciesManagedByRole[].SpeciesTypeId</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].SpeciesTypeId</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].GroupMarkStartDate</t>
+  </si>
+  <si>
+    <t>SamHerdDocument(PartyId)[].GroupMarkEndDate</t>
+  </si>
+  <si>
+    <t>DERIVED DATA</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Herdmark</t>
+  </si>
+  <si>
+    <t>CountyParishHoldingHerd</t>
+  </si>
+  <si>
+    <t>PartyId *</t>
+  </si>
+  <si>
+    <t>HoldingIdentifier *</t>
+  </si>
+  <si>
+    <t>RoleTypeId *</t>
+  </si>
+  <si>
+    <t>IsHolder *</t>
+  </si>
+  <si>
+    <t>Herdmark *</t>
+  </si>
+  <si>
+    <t>CountyParishHoldingHerd *</t>
+  </si>
+  <si>
+    <t>12/345/6789/01</t>
+  </si>
+  <si>
+    <t>SiteGroupMarkRelationshipDocument</t>
+  </si>
+  <si>
+    <t>SamHerdDocument</t>
+  </si>
+  <si>
+    <t>ProductionUsageId *</t>
+  </si>
+  <si>
+    <t>Derived by Party Roles from matching Herds</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Months</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -758,17 +867,27 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -818,7 +937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -871,6 +990,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1187,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1212,19 +1346,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -1236,33 +1370,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1280,431 +1414,531 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
+      <c r="A8" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
+      <c r="A10" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>37</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E17" s="18"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>32</v>
-      </c>
+    <row r="18" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="B19" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="6"/>
+        <v>121</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F19" s="7" t="s">
-        <v>134</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="4">
-        <v>25962203</v>
-      </c>
-      <c r="F24" s="4">
-        <v>25962203</v>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="E25" s="4">
-        <v>399568</v>
+        <v>25962203</v>
       </c>
       <c r="F25" s="4">
-        <v>399568</v>
+        <v>25962203</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E26" s="4">
-        <v>579087</v>
+        <v>399568</v>
       </c>
       <c r="F26" s="4">
-        <v>579087</v>
+        <v>399568</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="E27" s="4">
+        <v>579087</v>
+      </c>
+      <c r="F27" s="4">
+        <v>579087</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>20</v>
+        <v>180</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>39</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E30" s="18"/>
       <c r="F30" s="18"/>
     </row>
-    <row r="31" spans="1:6" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="E31" s="7" t="s">
+    <row r="31" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="F32" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:6" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="B41" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="3" t="s">
+    </row>
+    <row r="44" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="F47" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B37" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
-      <c r="B38" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="42" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="7"/>
-    </row>
-    <row r="44" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F44" s="7"/>
-    </row>
-    <row r="47" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="6"/>
+      <c r="B48" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+    </row>
+    <row r="52" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F52" s="7"/>
+    </row>
+    <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F54" s="7"/>
+    </row>
+    <row r="57" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F57" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1712,400 +1946,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF6CC05-8C87-45EE-8114-6B59C4D3ABC0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C839C088-4F6A-415F-B277-CCE418652376}">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="36.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="39.26953125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="38.81640625" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="37.54296875" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="E2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="11"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="11"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="9"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="E6" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C839C088-4F6A-415F-B277-CCE418652376}">
-  <dimension ref="A1:F40"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33:F34"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2127,19 +1972,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -2151,33 +1996,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2190,7 +2035,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -2203,471 +2048,491 @@
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>76</v>
-      </c>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>78</v>
+      <c r="E16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>167</v>
+      <c r="A17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>58</v>
+      <c r="E17" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>168</v>
+      <c r="A18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>90</v>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7" t="s">
-        <v>134</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="B25" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25" s="7"/>
+        <v>158</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F25" s="7" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="4">
+        <v>25962203</v>
+      </c>
+      <c r="F31" s="4">
+        <v>25962203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="4">
-        <v>25962203</v>
-      </c>
-      <c r="F29" s="4">
-        <v>25962203</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="E31" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
+      <c r="B32" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="E33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="E34" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="B35" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="6" t="s">
-        <v>142</v>
+        <v>167</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="E36" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B37" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B39" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B40" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>35</v>
+        <v>170</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B41" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E6 E15:F15" numberStoredAsText="1"/>
+    <ignoredError sqref="E6 E16:F16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA66AAD5-BDC2-41E6-A820-5F761A54ABFC}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A14" sqref="A14:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.6328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="58.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.08984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="36.36328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.08984375" style="3" customWidth="1"/>
     <col min="4" max="4" width="3.1796875" style="3" customWidth="1"/>
     <col min="5" max="5" width="36.6328125" style="4" customWidth="1"/>
     <col min="6" max="6" width="36.26953125" style="3" customWidth="1"/>
@@ -2682,19 +2547,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -2706,33 +2571,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2745,7 +2610,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -2757,59 +2622,233 @@
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>64</v>
+      <c r="A8" s="11" t="s">
+        <v>217</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="E9" s="7" t="s">
+    <row r="11" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F17" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>35</v>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2820,12 +2859,442 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF6CC05-8C87-45EE-8114-6B59C4D3ABC0}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.6328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="2.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="38.81640625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="37.54296875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="E2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E6 E24:F24" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454A6389-3CAC-4BFC-B100-395F08EF1093}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2836,94 +3305,102 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -2931,10 +3408,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Persistance for gold data completed
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBECAEB-B070-4E55-8EAE-54E5AAC7C9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6D1332-DFE7-4107-9F19-931258E2B281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" firstSheet="1" activeTab="4" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="11590" yWindow="1700" windowWidth="25980" windowHeight="18670" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Site Party Role Relations" sheetId="9" r:id="rId3"/>
     <sheet name="Site Group Mark Relations" sheetId="7" r:id="rId4"/>
     <sheet name="LOVs Required" sheetId="5" r:id="rId5"/>
+    <sheet name="TODOs" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="248">
   <si>
     <t>Source</t>
   </si>
@@ -804,6 +805,60 @@
   </si>
   <si>
     <t>Months</t>
+  </si>
+  <si>
+    <t>Ensure last updated date is taken from raw into silver</t>
+  </si>
+  <si>
+    <t>Add created date to gold</t>
+  </si>
+  <si>
+    <t>Species[].Id</t>
+  </si>
+  <si>
+    <t>Species[].Code</t>
+  </si>
+  <si>
+    <t>Species[].Name</t>
+  </si>
+  <si>
+    <t>BEEF</t>
+  </si>
+  <si>
+    <t>SiteActivities[].Id</t>
+  </si>
+  <si>
+    <t>SiteActivities[].Activity</t>
+  </si>
+  <si>
+    <t>SiteActivities[].Description</t>
+  </si>
+  <si>
+    <t>SiteActivities[].StartDate</t>
+  </si>
+  <si>
+    <t>SiteActivities[].EndDate</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>Ensure that only non Deleted records are exposed in API</t>
+  </si>
+  <si>
+    <t>Use Deleted flag instead of orphans CTS</t>
+  </si>
+  <si>
+    <t>Use Deleted flag instead of orphans SAM Silver</t>
+  </si>
+  <si>
+    <t>Use Deleted flag instead of orphans SAM Gold</t>
+  </si>
+  <si>
+    <t>Exclude all deleted items from relationship types</t>
+  </si>
+  <si>
+    <t>Create stubs for calling Odata API with selects</t>
   </si>
 </sst>
 </file>
@@ -1321,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1877,68 +1932,139 @@
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
     </row>
-    <row r="45" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="21" t="s">
+    <row r="45" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="B45" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="11"/>
+      <c r="B46" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="11"/>
+      <c r="B47" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-    </row>
-    <row r="46" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C46" s="10" t="s">
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+    </row>
+    <row r="52" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B47" s="3" t="s">
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C54" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="E54" s="9"/>
+      <c r="F54" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="6"/>
-      <c r="B48" s="3" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="6"/>
+      <c r="B55" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C55" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="52" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F52" s="7"/>
-    </row>
-    <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F54" s="7"/>
-    </row>
-    <row r="57" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="7"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+    </row>
+    <row r="59" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F59" s="7"/>
+    </row>
+    <row r="61" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F61" s="7"/>
+    </row>
+    <row r="64" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F64" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1949,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C839C088-4F6A-415F-B277-CCE418652376}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2525,7 +2651,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F15"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2864,7 +2990,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3293,7 +3419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454A6389-3CAC-4BFC-B100-395F08EF1093}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -3418,4 +3544,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A042D0B7-B54D-4053-AE08-00600F5C98ED}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="55.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implementation of the Insert Sam Holding Gold mappings step for sites and parties (#61)
* Mappings for gold added to domain and documents.

* CTS Silver data happy

* Persistance for gold data completed

---------

Co-authored-by: Mark Gent <Mark.Gent@homesengland.gov.uk>
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBECAEB-B070-4E55-8EAE-54E5AAC7C9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6D1332-DFE7-4107-9F19-931258E2B281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" firstSheet="1" activeTab="4" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="11590" yWindow="1700" windowWidth="25980" windowHeight="18670" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Site Party Role Relations" sheetId="9" r:id="rId3"/>
     <sheet name="Site Group Mark Relations" sheetId="7" r:id="rId4"/>
     <sheet name="LOVs Required" sheetId="5" r:id="rId5"/>
+    <sheet name="TODOs" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="248">
   <si>
     <t>Source</t>
   </si>
@@ -804,6 +805,60 @@
   </si>
   <si>
     <t>Months</t>
+  </si>
+  <si>
+    <t>Ensure last updated date is taken from raw into silver</t>
+  </si>
+  <si>
+    <t>Add created date to gold</t>
+  </si>
+  <si>
+    <t>Species[].Id</t>
+  </si>
+  <si>
+    <t>Species[].Code</t>
+  </si>
+  <si>
+    <t>Species[].Name</t>
+  </si>
+  <si>
+    <t>BEEF</t>
+  </si>
+  <si>
+    <t>SiteActivities[].Id</t>
+  </si>
+  <si>
+    <t>SiteActivities[].Activity</t>
+  </si>
+  <si>
+    <t>SiteActivities[].Description</t>
+  </si>
+  <si>
+    <t>SiteActivities[].StartDate</t>
+  </si>
+  <si>
+    <t>SiteActivities[].EndDate</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>Ensure that only non Deleted records are exposed in API</t>
+  </si>
+  <si>
+    <t>Use Deleted flag instead of orphans CTS</t>
+  </si>
+  <si>
+    <t>Use Deleted flag instead of orphans SAM Silver</t>
+  </si>
+  <si>
+    <t>Use Deleted flag instead of orphans SAM Gold</t>
+  </si>
+  <si>
+    <t>Exclude all deleted items from relationship types</t>
+  </si>
+  <si>
+    <t>Create stubs for calling Odata API with selects</t>
   </si>
 </sst>
 </file>
@@ -1321,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1877,68 +1932,139 @@
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
     </row>
-    <row r="45" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="21" t="s">
+    <row r="45" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="B45" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="11"/>
+      <c r="B46" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="11"/>
+      <c r="B47" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-    </row>
-    <row r="46" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C46" s="10" t="s">
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+    </row>
+    <row r="52" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B47" s="3" t="s">
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C54" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="E54" s="9"/>
+      <c r="F54" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="6"/>
-      <c r="B48" s="3" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="6"/>
+      <c r="B55" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C55" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="52" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F52" s="7"/>
-    </row>
-    <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F54" s="7"/>
-    </row>
-    <row r="57" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="7"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+    </row>
+    <row r="59" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F59" s="7"/>
+    </row>
+    <row r="61" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F61" s="7"/>
+    </row>
+    <row r="64" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F64" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1949,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C839C088-4F6A-415F-B277-CCE418652376}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2525,7 +2651,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F15"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2864,7 +2990,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3293,7 +3419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454A6389-3CAC-4BFC-B100-395F08EF1093}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -3418,4 +3544,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A042D0B7-B54D-4053-AE08-00600F5C98ED}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="55.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implementation of the Insert Sam Holding Gold mappings step for sites and parties (#65)
* Added stubs to the client for scanning

* Gold mappings wip

* Using created and updated dates from bridge side.

* Gold wip

* linting

---------

Co-authored-by: Mark Gent <Mark.Gent@homesengland.gov.uk>
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6D1332-DFE7-4107-9F19-931258E2B281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802255AE-AA2F-43F9-BA2D-2530AE4F35F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11590" yWindow="1700" windowWidth="25980" windowHeight="18670" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="3" activeTab="6" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Site Group Mark Relations" sheetId="7" r:id="rId4"/>
     <sheet name="LOVs Required" sheetId="5" r:id="rId5"/>
     <sheet name="TODOs" sheetId="11" r:id="rId6"/>
+    <sheet name="Import Strategy" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -115,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="280">
   <si>
     <t>Source</t>
   </si>
@@ -859,13 +860,109 @@
   </si>
   <si>
     <t>Create stubs for calling Odata API with selects</t>
+  </si>
+  <si>
+    <t>Add communications to gold role maps</t>
+  </si>
+  <si>
+    <t>Holder vs Party concerns</t>
+  </si>
+  <si>
+    <t>Bulk</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Holding</t>
+  </si>
+  <si>
+    <t>CPH</t>
+  </si>
+  <si>
+    <t>Holder</t>
+  </si>
+  <si>
+    <t>CPHS</t>
+  </si>
+  <si>
+    <t>12/345/6789,12/345/7890</t>
+  </si>
+  <si>
+    <t>Herd</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>CPHH</t>
+  </si>
+  <si>
+    <t>OwnerPartyIds</t>
+  </si>
+  <si>
+    <t>KeeperPartyIds</t>
+  </si>
+  <si>
+    <t>C1000001,C1000002</t>
+  </si>
+  <si>
+    <t>Keys</t>
+  </si>
+  <si>
+    <t>Examples</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
+  </si>
+  <si>
+    <t>Depends upon</t>
+  </si>
+  <si>
+    <t>Dependants</t>
+  </si>
+  <si>
+    <t>Parties</t>
+  </si>
+  <si>
+    <t>Ensure the holder imported 1st is included in Site Parties</t>
+  </si>
+  <si>
+    <t>Holding changed</t>
+  </si>
+  <si>
+    <t>Herds</t>
+  </si>
+  <si>
+    <t>Holders</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Parties</t>
+  </si>
+  <si>
+    <t>Herd changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Unique CPH</t>
+  </si>
+  <si>
+    <t>Holder changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Each CPH in CphList</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - CPH</t>
+  </si>
+  <si>
+    <t>Party changed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -944,6 +1041,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -992,7 +1096,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1062,6 +1166,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1378,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2075,7 +2187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C839C088-4F6A-415F-B277-CCE418652376}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -3548,52 +3660,318 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A042D0B7-B54D-4053-AE08-00600F5C98ED}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="25" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="25" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="25" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="25" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="25" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="25" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="25" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="25" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C08BCD-5565-4A1A-A7FC-55BC9438C9E6}">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="36.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="1.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E2" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E3" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E5" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E6" s="28"/>
+      <c r="F6" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E7" s="28"/>
+      <c r="F7" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E9" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E11" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>254</v>
+      </c>
+      <c r="F14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>257</v>
+      </c>
+      <c r="F16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E22" t="s">
+        <v>278</v>
+      </c>
+      <c r="F22" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E34" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E35" t="s">
+        <v>277</v>
+      </c>
+      <c r="F35" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F38" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F39" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E41" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to gold map docs
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802255AE-AA2F-43F9-BA2D-2530AE4F35F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248ED13A-61A1-4002-AF01-DCDBA86BF1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="3" activeTab="6" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="470" yWindow="3220" windowWidth="28530" windowHeight="17620" firstSheet="3" activeTab="6" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="300">
   <si>
     <t>Source</t>
   </si>
@@ -868,12 +868,6 @@
     <t>Holder vs Party concerns</t>
   </si>
   <si>
-    <t>Bulk</t>
-  </si>
-  <si>
-    <t>Daily</t>
-  </si>
-  <si>
     <t>Holding</t>
   </si>
   <si>
@@ -913,49 +907,115 @@
     <t>Examples</t>
   </si>
   <si>
-    <t>Dependencies</t>
-  </si>
-  <si>
-    <t>Depends upon</t>
-  </si>
-  <si>
-    <t>Dependants</t>
-  </si>
-  <si>
-    <t>Parties</t>
-  </si>
-  <si>
     <t>Ensure the holder imported 1st is included in Site Parties</t>
   </si>
   <si>
     <t>Holding changed</t>
   </si>
   <si>
-    <t>Herds</t>
-  </si>
-  <si>
-    <t>Holders</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Parties</t>
   </si>
   <si>
     <t>Herd changed</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Unique CPH</t>
-  </si>
-  <si>
     <t>Holder changed</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Each CPH in CphList</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - CPH</t>
-  </si>
-  <si>
     <t>Party changed</t>
+  </si>
+  <si>
+    <t>Import strategies</t>
+  </si>
+  <si>
+    <t>Bulk import strategy</t>
+  </si>
+  <si>
+    <t>Daily change strategy</t>
+  </si>
+  <si>
+    <t>Holdings</t>
+  </si>
+  <si>
+    <t>For each CPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Distinct CPH numbers extracted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Repeat Bulk Holdings strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Holding by CPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Herds by CPH(H)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Holder by CPHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Has a (matching PartyId) holder record changed too?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - If so, discard (Holder will pick up change)</t>
+  </si>
+  <si>
+    <t>Aggegate Parties and Holders</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - If not, continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Sam Party</t>
+  </si>
+  <si>
+    <t>Use Sam Party as base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - Find herd where owner or keeper id matches (PartyId) and also changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - If Sam Holder (matching PartyId) present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Append inferred Holder role. </t>
+  </si>
+  <si>
+    <t>Check name, communications &amp; address details.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           - If present discard (Her will pick up change)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Sam Holder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           - If not, use PartyId to find existing related CPH numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - If Holder has no associated Party, then use Holder as base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - Else discard</t>
+  </si>
+  <si>
+    <t>To Silver as is</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Distinct CPH numbers extracted from </t>
+  </si>
+  <si>
+    <t>To Gold as is</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Check for CPH numbers that have been removed</t>
+  </si>
+  <si>
+    <t>For each CPH orphan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Remove site party relationships</t>
   </si>
 </sst>
 </file>
@@ -3720,7 +3780,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -3730,248 +3790,269 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C08BCD-5565-4A1A-A7FC-55BC9438C9E6}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="1.90625" customWidth="1"/>
+    <col min="1" max="1" width="53.81640625" customWidth="1"/>
+    <col min="3" max="3" width="53.90625" customWidth="1"/>
+    <col min="4" max="4" width="67.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>263</v>
-      </c>
-      <c r="G1" s="30" t="s">
+      <c r="B2" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E2" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E3" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E4" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E5" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E6" s="28"/>
-      <c r="F6" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E7" s="28"/>
-      <c r="F7" s="28" t="s">
-        <v>261</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E9" s="26" t="s">
+      <c r="E13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" t="s">
+        <v>274</v>
+      </c>
+      <c r="E14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>273</v>
+      </c>
+      <c r="D16" t="s">
+        <v>266</v>
+      </c>
+      <c r="E16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" t="s">
+        <v>274</v>
+      </c>
+      <c r="E17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E11" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>266</v>
-      </c>
-      <c r="G11" s="30" t="s">
+      <c r="D19" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>278</v>
+      </c>
+      <c r="D20" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>283</v>
+      </c>
+      <c r="B23" t="s">
+        <v>284</v>
+      </c>
+      <c r="D23" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>286</v>
+      </c>
+      <c r="B24" t="s">
+        <v>287</v>
+      </c>
+      <c r="C24" t="s">
+        <v>288</v>
+      </c>
+      <c r="D24" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" t="s">
+        <v>291</v>
+      </c>
+      <c r="E25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>292</v>
+      </c>
+      <c r="E26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E12" t="s">
-        <v>252</v>
-      </c>
-      <c r="F12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F13" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E14" t="s">
-        <v>254</v>
-      </c>
-      <c r="F14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E15" t="s">
-        <v>258</v>
-      </c>
-      <c r="F15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E16" t="s">
-        <v>257</v>
-      </c>
-      <c r="F16" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="26" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E21" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E22" t="s">
-        <v>278</v>
-      </c>
-      <c r="F22" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F23" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F24" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F25" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>294</v>
+      </c>
+      <c r="D29" t="s">
+        <v>295</v>
+      </c>
+      <c r="E29" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E27" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E28" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>296</v>
+      </c>
+      <c r="E30" t="s">
         <v>275</v>
       </c>
-      <c r="F28" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F29" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F30" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F31" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F32" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E34" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E35" t="s">
-        <v>277</v>
-      </c>
-      <c r="F35" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="F36" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="F37" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="F38" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="F39" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E41" t="s">
-        <v>279</v>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>297</v>
+      </c>
+      <c r="E31" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E32" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gold maps doc saved
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3EC631-0A00-462B-BC3E-15352A0D6E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359D3E0B-ADC1-47CF-BA52-759E8ECEB414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="740" windowWidth="23300" windowHeight="19890" firstSheet="2" activeTab="5" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="2610" yWindow="1570" windowWidth="26100" windowHeight="19230" firstSheet="2" activeTab="5" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="287">
   <si>
     <t>Source</t>
   </si>
@@ -859,51 +859,6 @@
     <t>Create stubs for calling Odata API with selects</t>
   </si>
   <si>
-    <t>Holder vs Party concerns</t>
-  </si>
-  <si>
-    <t>Holding</t>
-  </si>
-  <si>
-    <t>CPH</t>
-  </si>
-  <si>
-    <t>Holder</t>
-  </si>
-  <si>
-    <t>CPHS</t>
-  </si>
-  <si>
-    <t>12/345/6789,12/345/7890</t>
-  </si>
-  <si>
-    <t>Herd</t>
-  </si>
-  <si>
-    <t>Party</t>
-  </si>
-  <si>
-    <t>CPHH</t>
-  </si>
-  <si>
-    <t>OwnerPartyIds</t>
-  </si>
-  <si>
-    <t>KeeperPartyIds</t>
-  </si>
-  <si>
-    <t>C1000001,C1000002</t>
-  </si>
-  <si>
-    <t>Keys</t>
-  </si>
-  <si>
-    <t>Examples</t>
-  </si>
-  <si>
-    <t>Ensure the holder imported 1st is included in Site Parties</t>
-  </si>
-  <si>
     <t>Holding changed</t>
   </si>
   <si>
@@ -919,9 +874,6 @@
     <t>Party changed</t>
   </si>
   <si>
-    <t>Import strategies</t>
-  </si>
-  <si>
     <t>Bulk import strategy</t>
   </si>
   <si>
@@ -976,9 +928,6 @@
     <t xml:space="preserve">Append inferred Holder role. </t>
   </si>
   <si>
-    <t>Check name, communications &amp; address details.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Sam Holder</t>
   </si>
   <si>
@@ -1015,9 +964,6 @@
     <t>RM</t>
   </si>
   <si>
-    <t>Remove Holder Scan and Import code</t>
-  </si>
-  <si>
     <t>Add step 1 to purge DB</t>
   </si>
   <si>
@@ -1025,6 +971,12 @@
   </si>
   <si>
     <t xml:space="preserve">           - If present discard (Herd will pick up change)</t>
+  </si>
+  <si>
+    <t>Remove SilverPartyRoles</t>
+  </si>
+  <si>
+    <t>Remove GoldSiteGroupMarks</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1236,12 +1188,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2013,7 +1959,7 @@
         <v>103</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="F36" s="18"/>
     </row>
@@ -2060,7 +2006,7 @@
         <v>103</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="F40" s="18"/>
     </row>
@@ -3729,269 +3675,206 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C08BCD-5565-4A1A-A7FC-55BC9438C9E6}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="53.81640625" customWidth="1"/>
-    <col min="3" max="3" width="53.90625" customWidth="1"/>
+    <col min="3" max="3" width="4.81640625" customWidth="1"/>
     <col min="4" max="4" width="67.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="30" t="s">
+      <c r="A1" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>249</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28" t="s">
-        <v>256</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="26" t="s">
-        <v>267</v>
-      </c>
+      <c r="D10" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30" t="s">
-        <v>269</v>
-      </c>
+      <c r="D11" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D13" t="s">
-        <v>262</v>
-      </c>
-      <c r="E13" t="s">
-        <v>271</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="B13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D14" t="s">
-        <v>272</v>
-      </c>
-      <c r="E14" t="s">
-        <v>273</v>
+        <v>268</v>
+      </c>
+      <c r="B14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>271</v>
-      </c>
-      <c r="D16" t="s">
-        <v>264</v>
-      </c>
-      <c r="E16" t="s">
-        <v>271</v>
+        <v>272</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>274</v>
-      </c>
-      <c r="D17" t="s">
-        <v>272</v>
-      </c>
-      <c r="E17" t="s">
         <v>273</v>
       </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>275</v>
-      </c>
+      <c r="D18" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>263</v>
-      </c>
-      <c r="D19" t="s">
-        <v>266</v>
+        <v>274</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>276</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="15"/>
+      <c r="E20" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21" s="15" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D21" t="s">
+      <c r="E21" s="15" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="D22" s="15"/>
+      <c r="E22" s="15" t="s">
         <v>279</v>
-      </c>
-      <c r="D22" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>281</v>
-      </c>
-      <c r="B23" t="s">
-        <v>282</v>
-      </c>
-      <c r="D23" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>284</v>
-      </c>
-      <c r="B24" t="s">
-        <v>285</v>
-      </c>
-      <c r="C24" t="s">
-        <v>286</v>
-      </c>
-      <c r="D24" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>287</v>
-      </c>
-      <c r="D25" t="s">
-        <v>288</v>
-      </c>
-      <c r="E25" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>289</v>
-      </c>
-      <c r="E26" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D28" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>291</v>
-      </c>
-      <c r="D29" t="s">
-        <v>292</v>
-      </c>
-      <c r="E29" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>293</v>
-      </c>
-      <c r="E30" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D31" t="s">
-        <v>294</v>
-      </c>
-      <c r="E31" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E32" t="s">
-        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -4004,7 +3887,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4049,29 +3932,27 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>247</v>
-      </c>
-    </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>261</v>
+      <c r="A11" s="15"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature/ulitp 3299 update sam data (#69)
* WIP

* Updates to gold map docs

* Added test scenario to prove import mappings

* WIP

* Gold sites and parties updated and orphans trimmed.

* Updated herd, holder daily scans to use holding id.

* Gold maps doc saved

* Merger from dev into FB

* Updated SAM Daily scans

* Merge CTS and SAM approaches

* Linting

* Corrected SAM integration tests

---------

Co-authored-by: Mark Gent <Mark.Gent@homesengland.gov.uk>
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802255AE-AA2F-43F9-BA2D-2530AE4F35F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359D3E0B-ADC1-47CF-BA52-759E8ECEB414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="3" activeTab="6" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="2610" yWindow="1570" windowWidth="26100" windowHeight="19230" firstSheet="2" activeTab="5" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Site Party Role Relations" sheetId="9" r:id="rId3"/>
     <sheet name="Site Group Mark Relations" sheetId="7" r:id="rId4"/>
     <sheet name="LOVs Required" sheetId="5" r:id="rId5"/>
-    <sheet name="TODOs" sheetId="11" r:id="rId6"/>
-    <sheet name="Import Strategy" sheetId="12" r:id="rId7"/>
+    <sheet name="Import Strategy" sheetId="12" r:id="rId6"/>
+    <sheet name="TODOs" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="287">
   <si>
     <t>Source</t>
   </si>
@@ -229,9 +229,6 @@
     <t>PERMANENT</t>
   </si>
   <si>
-    <t>TB-AFU</t>
-  </si>
-  <si>
     <t>TB</t>
   </si>
   <si>
@@ -862,100 +859,124 @@
     <t>Create stubs for calling Odata API with selects</t>
   </si>
   <si>
-    <t>Add communications to gold role maps</t>
-  </si>
-  <si>
-    <t>Holder vs Party concerns</t>
-  </si>
-  <si>
-    <t>Bulk</t>
-  </si>
-  <si>
-    <t>Daily</t>
-  </si>
-  <si>
-    <t>Holding</t>
-  </si>
-  <si>
-    <t>CPH</t>
-  </si>
-  <si>
-    <t>Holder</t>
-  </si>
-  <si>
-    <t>CPHS</t>
-  </si>
-  <si>
-    <t>12/345/6789,12/345/7890</t>
-  </si>
-  <si>
-    <t>Herd</t>
-  </si>
-  <si>
-    <t>Party</t>
-  </si>
-  <si>
-    <t>CPHH</t>
-  </si>
-  <si>
-    <t>OwnerPartyIds</t>
-  </si>
-  <si>
-    <t>KeeperPartyIds</t>
-  </si>
-  <si>
-    <t>C1000001,C1000002</t>
-  </si>
-  <si>
-    <t>Keys</t>
-  </si>
-  <si>
-    <t>Examples</t>
-  </si>
-  <si>
-    <t>Dependencies</t>
-  </si>
-  <si>
-    <t>Depends upon</t>
-  </si>
-  <si>
-    <t>Dependants</t>
-  </si>
-  <si>
-    <t>Parties</t>
-  </si>
-  <si>
-    <t>Ensure the holder imported 1st is included in Site Parties</t>
-  </si>
-  <si>
     <t>Holding changed</t>
   </si>
   <si>
-    <t>Herds</t>
-  </si>
-  <si>
-    <t>Holders</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Parties</t>
   </si>
   <si>
     <t>Herd changed</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Unique CPH</t>
-  </si>
-  <si>
     <t>Holder changed</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Each CPH in CphList</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - CPH</t>
-  </si>
-  <si>
     <t>Party changed</t>
+  </si>
+  <si>
+    <t>Bulk import strategy</t>
+  </si>
+  <si>
+    <t>Daily change strategy</t>
+  </si>
+  <si>
+    <t>Holdings</t>
+  </si>
+  <si>
+    <t>For each CPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Distinct CPH numbers extracted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Repeat Bulk Holdings strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Holding by CPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Herds by CPH(H)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Holder by CPHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Has a (matching PartyId) holder record changed too?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - If so, discard (Holder will pick up change)</t>
+  </si>
+  <si>
+    <t>Aggegate Parties and Holders</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - If not, continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Sam Party</t>
+  </si>
+  <si>
+    <t>Use Sam Party as base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - Find herd where owner or keeper id matches (PartyId) and also changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - If Sam Holder (matching PartyId) present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Append inferred Holder role. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Sam Holder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           - If not, use PartyId to find existing related CPH numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - If Holder has no associated Party, then use Holder as base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - Else discard</t>
+  </si>
+  <si>
+    <t>To Silver as is</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Distinct CPH numbers extracted from </t>
+  </si>
+  <si>
+    <t>To Gold as is</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Check for CPH numbers that have been removed</t>
+  </si>
+  <si>
+    <t>For each CPH orphan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Remove site party relationships</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>Add step 1 to purge DB</t>
+  </si>
+  <si>
+    <t>Add run on date for bulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           - If present discard (Herd will pick up change)</t>
+  </si>
+  <si>
+    <t>Remove SilverPartyRoles</t>
+  </si>
+  <si>
+    <t>Remove GoldSiteGroupMarks</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1167,12 +1188,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1490,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1522,10 +1537,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -1537,10 +1552,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
@@ -1549,21 +1564,21 @@
         <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="F5" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1582,10 +1597,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>24</v>
@@ -1596,22 +1611,22 @@
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>34</v>
@@ -1625,7 +1640,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>36</v>
@@ -1637,13 +1652,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1651,7 +1666,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>27</v>
@@ -1665,7 +1680,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>28</v>
@@ -1679,7 +1694,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>31</v>
@@ -1693,7 +1708,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>26</v>
@@ -1704,10 +1719,10 @@
     </row>
     <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
@@ -1717,7 +1732,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>35</v>
@@ -1729,10 +1744,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7" t="s">
@@ -1745,61 +1760,61 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1807,7 +1822,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E25" s="4">
         <v>25962203</v>
@@ -1860,30 +1875,30 @@
     </row>
     <row r="29" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
@@ -1893,7 +1908,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>32</v>
@@ -1907,7 +1922,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>33</v>
@@ -1918,20 +1933,20 @@
     </row>
     <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
@@ -1941,10 +1956,10 @@
         <v>18</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>37</v>
+        <v>281</v>
       </c>
       <c r="F36" s="18"/>
     </row>
@@ -1953,10 +1968,10 @@
         <v>20</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>30</v>
@@ -1965,20 +1980,20 @@
     </row>
     <row r="38" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B39" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -1988,10 +2003,10 @@
         <v>19</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>38</v>
+        <v>280</v>
       </c>
       <c r="F40" s="18"/>
     </row>
@@ -2000,25 +2015,25 @@
         <v>21</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>106</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7" t="s">
         <v>30</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
@@ -2028,28 +2043,28 @@
         <v>22</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="7" t="s">
@@ -2059,34 +2074,34 @@
     <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11"/>
       <c r="B46" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11"/>
       <c r="B47" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>30</v>
@@ -2094,38 +2109,38 @@
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B49" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B50" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B51" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
     </row>
     <row r="52" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B52" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
@@ -2139,20 +2154,20 @@
         <v>0</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
       <c r="B55" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>143</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="7"/>
@@ -2219,10 +2234,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -2234,10 +2249,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
@@ -2246,21 +2261,21 @@
         <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="F5" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2273,7 +2288,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -2286,250 +2301,250 @@
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>134</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>35</v>
@@ -2537,13 +2552,13 @@
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>30</v>
@@ -2554,55 +2569,55 @@
     </row>
     <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -2615,10 +2630,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>32</v>
@@ -2629,10 +2644,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C33" s="8"/>
       <c r="E33" s="4" t="s">
@@ -2644,21 +2659,21 @@
     </row>
     <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>30</v>
@@ -2669,33 +2684,33 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C36" s="6"/>
       <c r="E36" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>30</v>
@@ -2706,28 +2721,28 @@
     </row>
     <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B39" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B40" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B41" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>32</v>
@@ -2738,10 +2753,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B42" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>33</v>
@@ -2794,10 +2809,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -2809,10 +2824,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
@@ -2821,21 +2836,21 @@
         <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="F5" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2848,7 +2863,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -2861,52 +2876,52 @@
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>24</v>
@@ -2917,16 +2932,16 @@
     </row>
     <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -2934,17 +2949,17 @@
         <v>0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>30</v>
@@ -2955,34 +2970,34 @@
     </row>
     <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>32</v>
@@ -2993,10 +3008,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>33</v>
@@ -3007,13 +3022,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>30</v>
@@ -3021,10 +3036,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>30</v>
@@ -3035,38 +3050,38 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>32</v>
@@ -3077,10 +3092,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>33</v>
@@ -3132,10 +3147,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="13" t="s">
@@ -3147,7 +3162,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
@@ -3156,18 +3171,18 @@
         <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="F5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -3177,7 +3192,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -3191,88 +3206,88 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -3285,26 +3300,26 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>30</v>
@@ -3316,25 +3331,25 @@
     <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>30</v>
@@ -3345,26 +3360,26 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -3377,108 +3392,108 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -3491,10 +3506,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -3543,10 +3558,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>12</v>
@@ -3554,26 +3569,26 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -3581,10 +3596,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
         <v>90</v>
-      </c>
-      <c r="C6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -3592,42 +3607,42 @@
         <v>20</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -3635,10 +3650,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -3646,10 +3661,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3659,319 +3674,285 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C08BCD-5565-4A1A-A7FC-55BC9438C9E6}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="36.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="53.81640625" customWidth="1"/>
+    <col min="3" max="3" width="4.81640625" customWidth="1"/>
+    <col min="4" max="4" width="67.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>272</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>273</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D18" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>274</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>276</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D22" s="15"/>
+      <c r="E22" s="15" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A042D0B7-B54D-4053-AE08-00600F5C98ED}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>269</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C08BCD-5565-4A1A-A7FC-55BC9438C9E6}">
-  <dimension ref="A1:G41"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="36.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="1.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>263</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E2" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E3" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E4" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E5" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E6" s="28"/>
-      <c r="F6" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E7" s="28"/>
-      <c r="F7" s="28" t="s">
-        <v>261</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E9" s="26" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E11" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>266</v>
-      </c>
-      <c r="G11" s="30" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E12" t="s">
-        <v>252</v>
-      </c>
-      <c r="F12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F13" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E14" t="s">
-        <v>254</v>
-      </c>
-      <c r="F14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E15" t="s">
-        <v>258</v>
-      </c>
-      <c r="F15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E16" t="s">
-        <v>257</v>
-      </c>
-      <c r="F16" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="26" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E21" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E22" t="s">
-        <v>278</v>
-      </c>
-      <c r="F22" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F23" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F24" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F25" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E27" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E28" t="s">
-        <v>275</v>
-      </c>
-      <c r="F28" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F29" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F30" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F31" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F32" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E34" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E35" t="s">
-        <v>277</v>
-      </c>
-      <c r="F35" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="F36" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="F37" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="F38" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="F39" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E41" t="s">
-        <v>279</v>
+      <c r="A11" s="15"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to the Site premise type and activity type mappings.
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359D3E0B-ADC1-47CF-BA52-759E8ECEB414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255820FC-7E1E-45F9-AA0F-20A344EA7B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="1570" windowWidth="26100" windowHeight="19230" firstSheet="2" activeTab="5" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="9720" yWindow="270" windowWidth="22150" windowHeight="20210" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Site Group Mark Relations" sheetId="7" r:id="rId4"/>
     <sheet name="LOVs Required" sheetId="5" r:id="rId5"/>
     <sheet name="Import Strategy" sheetId="12" r:id="rId6"/>
-    <sheet name="TODOs" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -116,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="275">
   <si>
     <t>Source</t>
   </si>
@@ -805,12 +804,6 @@
     <t>Months</t>
   </si>
   <si>
-    <t>Ensure last updated date is taken from raw into silver</t>
-  </si>
-  <si>
-    <t>Add created date to gold</t>
-  </si>
-  <si>
     <t>Species[].Id</t>
   </si>
   <si>
@@ -841,24 +834,6 @@
     <t>Beef</t>
   </si>
   <si>
-    <t>Ensure that only non Deleted records are exposed in API</t>
-  </si>
-  <si>
-    <t>Use Deleted flag instead of orphans CTS</t>
-  </si>
-  <si>
-    <t>Use Deleted flag instead of orphans SAM Silver</t>
-  </si>
-  <si>
-    <t>Use Deleted flag instead of orphans SAM Gold</t>
-  </si>
-  <si>
-    <t>Exclude all deleted items from relationship types</t>
-  </si>
-  <si>
-    <t>Create stubs for calling Odata API with selects</t>
-  </si>
-  <si>
     <t>Holding changed</t>
   </si>
   <si>
@@ -964,26 +939,14 @@
     <t>RM</t>
   </si>
   <si>
-    <t>Add step 1 to purge DB</t>
-  </si>
-  <si>
-    <t>Add run on date for bulk</t>
-  </si>
-  <si>
     <t xml:space="preserve">           - If present discard (Herd will pick up change)</t>
-  </si>
-  <si>
-    <t>Remove SilverPartyRoles</t>
-  </si>
-  <si>
-    <t>Remove GoldSiteGroupMarks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1062,13 +1025,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1117,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1187,7 +1143,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1505,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1959,7 +1914,7 @@
         <v>103</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F36" s="18"/>
     </row>
@@ -2006,7 +1961,7 @@
         <v>103</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F40" s="18"/>
     </row>
@@ -2064,7 +2019,7 @@
         <v>185</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="7" t="s">
@@ -2074,7 +2029,7 @@
     <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11"/>
       <c r="B46" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>38</v>
@@ -2086,7 +2041,7 @@
     <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11"/>
       <c r="B47" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="9" t="s">
@@ -2098,7 +2053,7 @@
         <v>184</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E48" s="9" t="s">
         <v>39</v>
@@ -2109,25 +2064,25 @@
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B49" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B50" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B51" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>103</v>
@@ -2137,7 +2092,7 @@
     </row>
     <row r="52" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B52" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>103</v>
@@ -3677,7 +3632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C08BCD-5565-4A1A-A7FC-55BC9438C9E6}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -3689,35 +3644,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
-        <v>253</v>
+      <c r="A1" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>247</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -3726,233 +3681,155 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D11" s="15" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B13" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B14" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D18" s="15" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D21" s="15" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D22" s="15"/>
       <c r="E22" s="15" t="s">
-        <v>279</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A042D0B7-B54D-4053-AE08-00600F5C98ED}">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="55.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="25" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature/ulitp 3624 validate import (#75)
* Remove silver role maps from persistence for CTS

* Updated code to keep mapped data but remove from persistence.

* Removed silver role and gold group map relations from SAM persistence

* Updated to the Site premise type and activity type mappings.

* Updated gold data verifications for integration test

* Tests updated

* Linting

---------

Co-authored-by: Mark Gent <Mark.Gent@homesengland.gov.uk>
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-gold-attr-map.xlsx
+++ b/docs/data-maps/sam-gold-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359D3E0B-ADC1-47CF-BA52-759E8ECEB414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255820FC-7E1E-45F9-AA0F-20A344EA7B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="1570" windowWidth="26100" windowHeight="19230" firstSheet="2" activeTab="5" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="9720" yWindow="270" windowWidth="22150" windowHeight="20210" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holding" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Site Group Mark Relations" sheetId="7" r:id="rId4"/>
     <sheet name="LOVs Required" sheetId="5" r:id="rId5"/>
     <sheet name="Import Strategy" sheetId="12" r:id="rId6"/>
-    <sheet name="TODOs" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -116,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="275">
   <si>
     <t>Source</t>
   </si>
@@ -805,12 +804,6 @@
     <t>Months</t>
   </si>
   <si>
-    <t>Ensure last updated date is taken from raw into silver</t>
-  </si>
-  <si>
-    <t>Add created date to gold</t>
-  </si>
-  <si>
     <t>Species[].Id</t>
   </si>
   <si>
@@ -841,24 +834,6 @@
     <t>Beef</t>
   </si>
   <si>
-    <t>Ensure that only non Deleted records are exposed in API</t>
-  </si>
-  <si>
-    <t>Use Deleted flag instead of orphans CTS</t>
-  </si>
-  <si>
-    <t>Use Deleted flag instead of orphans SAM Silver</t>
-  </si>
-  <si>
-    <t>Use Deleted flag instead of orphans SAM Gold</t>
-  </si>
-  <si>
-    <t>Exclude all deleted items from relationship types</t>
-  </si>
-  <si>
-    <t>Create stubs for calling Odata API with selects</t>
-  </si>
-  <si>
     <t>Holding changed</t>
   </si>
   <si>
@@ -964,26 +939,14 @@
     <t>RM</t>
   </si>
   <si>
-    <t>Add step 1 to purge DB</t>
-  </si>
-  <si>
-    <t>Add run on date for bulk</t>
-  </si>
-  <si>
     <t xml:space="preserve">           - If present discard (Herd will pick up change)</t>
-  </si>
-  <si>
-    <t>Remove SilverPartyRoles</t>
-  </si>
-  <si>
-    <t>Remove GoldSiteGroupMarks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1062,13 +1025,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1117,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1187,7 +1143,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1505,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1959,7 +1914,7 @@
         <v>103</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F36" s="18"/>
     </row>
@@ -2006,7 +1961,7 @@
         <v>103</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F40" s="18"/>
     </row>
@@ -2064,7 +2019,7 @@
         <v>185</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="7" t="s">
@@ -2074,7 +2029,7 @@
     <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11"/>
       <c r="B46" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>38</v>
@@ -2086,7 +2041,7 @@
     <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11"/>
       <c r="B47" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="9" t="s">
@@ -2098,7 +2053,7 @@
         <v>184</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E48" s="9" t="s">
         <v>39</v>
@@ -2109,25 +2064,25 @@
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B49" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B50" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B51" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>103</v>
@@ -2137,7 +2092,7 @@
     </row>
     <row r="52" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B52" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>103</v>
@@ -3677,7 +3632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C08BCD-5565-4A1A-A7FC-55BC9438C9E6}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -3689,35 +3644,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
-        <v>253</v>
+      <c r="A1" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>247</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -3726,233 +3681,155 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D11" s="15" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B13" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B14" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D18" s="15" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D21" s="15" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D22" s="15"/>
       <c r="E22" s="15" t="s">
-        <v>279</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A042D0B7-B54D-4053-AE08-00600F5C98ED}">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="55.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="25" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>